<commit_message>
Practice with excell and python
</commit_message>
<xml_diff>
--- a/transactions2.xlsx
+++ b/transactions2.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
@@ -478,6 +478,11 @@
           <t xml:space="preserve">price </t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Correct price</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="3">
       <c r="A2" s="2" t="n">
@@ -519,6 +524,96 @@
       </c>
       <c r="D4" t="n">
         <v>7.155</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>David 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>David 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>David 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>David 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>David 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>David 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>David 12</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>David 13</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>David 14</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
practiced BarChart from pyxl
</commit_message>
<xml_diff>
--- a/transactions2.xlsx
+++ b/transactions2.xlsx
@@ -162,6 +162,90 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$D$2:$D$5</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -446,12 +530,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
@@ -616,6 +700,50 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>6</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7</v>
+      </c>
+      <c r="H16" t="n">
+        <v>8</v>
+      </c>
+      <c r="I16" t="n">
+        <v>9</v>
+      </c>
+      <c r="J16" t="n">
+        <v>10</v>
+      </c>
+      <c r="K16" t="n">
+        <v>11</v>
+      </c>
+      <c r="L16" t="n">
+        <v>12</v>
+      </c>
+      <c r="M16" t="n">
+        <v>13</v>
+      </c>
+      <c r="N16" t="n">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -628,5 +756,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>